<commit_message>
GPLIM-4712 add changes from discussion with users
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/ExternalLibraryMultiOrganismTest.xlsx
+++ b/mercury/src/test/resources/testdata/ExternalLibraryMultiOrganismTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="153">
   <si>
     <t>Sample Kit Shipping Information</t>
   </si>
@@ -503,6 +503,18 @@
   </si>
   <si>
     <t>sub-human</t>
+  </si>
+  <si>
+    <t>Sample Tube Barcode</t>
+  </si>
+  <si>
+    <t>4076255991</t>
+  </si>
+  <si>
+    <t>4076255992</t>
+  </si>
+  <si>
+    <t>4076255993</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1161,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="122">
+  <cellStyleXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1275,8 +1287,12 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1316,7 +1332,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="7" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="46" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="46" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="46" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="30" borderId="12" xfId="46" applyFill="1" applyBorder="1"/>
@@ -1403,7 +1418,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="122">
+  <cellStyles count="126">
     <cellStyle name="20% - Accent1 2" xfId="8"/>
     <cellStyle name="20% - Accent1 2 2" xfId="50"/>
     <cellStyle name="20% - Accent2 2" xfId="9"/>
@@ -1472,6 +1487,8 @@
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
     <cellStyle name="Good 2" xfId="31"/>
     <cellStyle name="Heading 1 2" xfId="32"/>
     <cellStyle name="Heading 2 2" xfId="33"/>
@@ -1505,6 +1522,8 @@
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="63"/>
     <cellStyle name="Input 2" xfId="36"/>
     <cellStyle name="Linked Cell 2" xfId="37"/>
@@ -1917,19 +1936,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L20" workbookViewId="0">
-      <selection activeCell="Z31" sqref="Z31"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.5" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="24.33203125" customWidth="1"/>
     <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" style="77" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="76" customWidth="1"/>
     <col min="11" max="11" width="30.33203125" customWidth="1"/>
     <col min="12" max="12" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="10.6640625" customWidth="1"/>
@@ -1938,31 +1958,31 @@
     <col min="22" max="22" width="14.5" customWidth="1"/>
     <col min="24" max="24" width="14.33203125" customWidth="1"/>
     <col min="25" max="25" width="13.1640625" customWidth="1"/>
-    <col min="26" max="26" width="17.6640625" style="39" customWidth="1"/>
-    <col min="27" max="27" width="13.6640625" style="39" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" style="38" customWidth="1"/>
+    <col min="27" max="27" width="13.6640625" style="38" customWidth="1"/>
     <col min="28" max="28" width="40.6640625" customWidth="1"/>
     <col min="29" max="32" width="40.83203125" customWidth="1"/>
-    <col min="33" max="33" width="31.5" style="39" customWidth="1"/>
+    <col min="33" max="33" width="31.5" style="38" customWidth="1"/>
     <col min="34" max="36" width="40.83203125" customWidth="1"/>
-    <col min="37" max="37" width="40.83203125" style="39" customWidth="1"/>
+    <col min="37" max="37" width="40.83203125" style="38" customWidth="1"/>
     <col min="38" max="38" width="40.83203125" customWidth="1"/>
     <col min="39" max="52" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" s="39" customFormat="1">
-      <c r="J1" s="77"/>
+    <row r="1" spans="2:28" s="38" customFormat="1">
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="2:28" ht="17" customHeight="1">
-      <c r="AA2" s="59"/>
+      <c r="AA2" s="58"/>
     </row>
     <row r="3" spans="2:28">
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="AA3" s="59"/>
+      <c r="AA3" s="58"/>
     </row>
     <row r="4" spans="2:28">
-      <c r="AA4" s="59"/>
+      <c r="AA4" s="58"/>
     </row>
     <row r="5" spans="2:28">
       <c r="B5" t="s">
@@ -1971,7 +1991,7 @@
       <c r="C5" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="AA5" s="59"/>
+      <c r="AA5" s="58"/>
     </row>
     <row r="6" spans="2:28">
       <c r="B6" t="s">
@@ -1980,7 +2000,7 @@
       <c r="C6" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="AA6" s="59"/>
+      <c r="AA6" s="58"/>
     </row>
     <row r="7" spans="2:28">
       <c r="B7" t="s">
@@ -1989,16 +2009,16 @@
       <c r="C7" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="AA7" s="59"/>
+      <c r="AA7" s="58"/>
     </row>
     <row r="8" spans="2:28">
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="58" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="AA8" s="59"/>
+      <c r="AA8" s="58"/>
     </row>
     <row r="9" spans="2:28">
       <c r="B9" t="s">
@@ -2007,18 +2027,18 @@
       <c r="C9" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="AA9" s="59"/>
+      <c r="AA9" s="58"/>
     </row>
     <row r="10" spans="2:28">
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="12"/>
-      <c r="AA10" s="59"/>
+      <c r="AA10" s="58"/>
     </row>
     <row r="11" spans="2:28">
       <c r="C11" s="3"/>
-      <c r="AA11" s="59"/>
+      <c r="AA11" s="58"/>
     </row>
     <row r="12" spans="2:28">
       <c r="B12" t="s">
@@ -2027,8 +2047,8 @@
       <c r="C12" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="AA12" s="59"/>
-      <c r="AB12" s="61" t="s">
+      <c r="AA12" s="58"/>
+      <c r="AB12" s="60" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2039,8 +2059,8 @@
       <c r="C13" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="AA13" s="59"/>
-      <c r="AB13" s="62" t="s">
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="61" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2048,11 +2068,11 @@
       <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="91" t="s">
+      <c r="C14" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="AA14" s="59"/>
-      <c r="AB14" s="62" t="s">
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="61" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2063,8 +2083,8 @@
       <c r="C15" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="62" t="s">
+      <c r="AA15" s="58"/>
+      <c r="AB15" s="61" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2072,11 +2092,11 @@
       <c r="B16" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="91" t="s">
+      <c r="C16" s="90" t="s">
         <v>140</v>
       </c>
-      <c r="AA16" s="59"/>
-      <c r="AB16" s="62" t="s">
+      <c r="AA16" s="58"/>
+      <c r="AB16" s="61" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2087,102 +2107,105 @@
       <c r="C17" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="AA17" s="59"/>
-      <c r="AB17" s="62"/>
+      <c r="AA17" s="58"/>
+      <c r="AB17" s="61"/>
     </row>
     <row r="18" spans="1:39">
       <c r="C18" s="13"/>
-      <c r="AA18" s="59"/>
-      <c r="AB18" s="62"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="61"/>
     </row>
     <row r="19" spans="1:39">
       <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="AA19" s="59"/>
-      <c r="AB19" s="63"/>
+      <c r="AA19" s="58"/>
+      <c r="AB19" s="62"/>
     </row>
     <row r="20" spans="1:39">
       <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="AA20" s="59"/>
-      <c r="AB20" s="63"/>
+      <c r="AA20" s="58"/>
+      <c r="AB20" s="62"/>
     </row>
     <row r="21" spans="1:39">
       <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="C21" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="AA21" s="59"/>
-      <c r="AB21" s="63"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="62"/>
     </row>
     <row r="22" spans="1:39">
       <c r="B22" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="AA22" s="59"/>
-      <c r="AB22" s="63"/>
+      <c r="AA22" s="58"/>
+      <c r="AB22" s="62"/>
     </row>
     <row r="23" spans="1:39">
       <c r="B23" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="AA23" s="59"/>
-      <c r="AB23" s="63"/>
+      <c r="AA23" s="58"/>
+      <c r="AB23" s="62"/>
     </row>
     <row r="24" spans="1:39" s="2" customFormat="1">
-      <c r="A24" s="39"/>
-      <c r="B24" s="58" t="s">
+      <c r="A24" s="38"/>
+      <c r="B24" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="J24" s="77"/>
-      <c r="Z24" s="39"/>
-      <c r="AA24" s="59"/>
-      <c r="AB24" s="63"/>
-      <c r="AG24" s="39"/>
-      <c r="AK24" s="39"/>
+      <c r="C24" s="48"/>
+      <c r="J24" s="76"/>
+      <c r="Z24" s="38"/>
+      <c r="AA24" s="58"/>
+      <c r="AB24" s="62"/>
+      <c r="AG24" s="38"/>
+      <c r="AK24" s="38"/>
     </row>
     <row r="25" spans="1:39" s="2" customFormat="1">
-      <c r="A25" s="39"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="49"/>
-      <c r="J25" s="77"/>
-      <c r="Z25" s="39"/>
-      <c r="AA25" s="59"/>
-      <c r="AB25" s="63"/>
-      <c r="AG25" s="39"/>
-      <c r="AK25" s="39"/>
+      <c r="C25" s="48"/>
+      <c r="J25" s="76"/>
+      <c r="Z25" s="38"/>
+      <c r="AA25" s="58"/>
+      <c r="AB25" s="62"/>
+      <c r="AG25" s="38"/>
+      <c r="AK25" s="38"/>
     </row>
     <row r="26" spans="1:39" s="2" customFormat="1">
-      <c r="A26" s="67" t="s">
+      <c r="A26" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="68"/>
-      <c r="C26" s="69"/>
-      <c r="J26" s="77"/>
-      <c r="Z26" s="39"/>
-      <c r="AA26" s="59"/>
-      <c r="AB26" s="63"/>
-      <c r="AG26" s="39"/>
-      <c r="AK26" s="39"/>
-    </row>
-    <row r="27" spans="1:39" s="33" customFormat="1" ht="78.75" customHeight="1">
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="J26" s="76"/>
+      <c r="Z26" s="38"/>
+      <c r="AA26" s="58"/>
+      <c r="AB26" s="62"/>
+      <c r="AG26" s="38"/>
+      <c r="AK26" s="38"/>
+    </row>
+    <row r="27" spans="1:39" s="32" customFormat="1" ht="78.75" customHeight="1">
+      <c r="A27" s="32" t="s">
+        <v>149</v>
+      </c>
       <c r="B27" s="5" t="s">
         <v>73</v>
       </c>
@@ -2204,10 +2227,10 @@
       <c r="H27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I27" s="94" t="s">
+      <c r="I27" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="J27" s="78" t="s">
+      <c r="J27" s="77" t="s">
         <v>22</v>
       </c>
       <c r="K27" s="5" t="s">
@@ -2255,90 +2278,90 @@
       <c r="Y27" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Z27" s="70" t="s">
+      <c r="Z27" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="AA27" s="60" t="s">
+      <c r="AA27" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="AB27" s="71" t="s">
+      <c r="AB27" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="AC27" s="60" t="s">
+      <c r="AC27" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="AD27" s="60" t="s">
+      <c r="AD27" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="AE27" s="60" t="s">
+      <c r="AE27" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="AF27" s="60" t="s">
+      <c r="AF27" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="AG27" s="66" t="s">
+      <c r="AG27" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="AH27" s="60" t="s">
+      <c r="AH27" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="AI27" s="60" t="s">
+      <c r="AI27" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="AJ27" s="60" t="s">
+      <c r="AJ27" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="AK27" s="60" t="s">
+      <c r="AK27" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="AL27" s="60" t="s">
+      <c r="AL27" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="AM27" s="60" t="s">
+      <c r="AM27" s="59" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:39" s="39" customFormat="1" ht="14">
-      <c r="A28" s="29">
-        <v>1</v>
-      </c>
-      <c r="B28" s="30" t="s">
+    <row r="28" spans="1:39" s="38" customFormat="1" ht="14">
+      <c r="A28" s="88" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="74"/>
-      <c r="E28" s="87" t="s">
+      <c r="D28" s="73"/>
+      <c r="E28" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87" t="s">
+      <c r="F28" s="86"/>
+      <c r="G28" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="H28" s="31" t="s">
+      <c r="H28" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="I28" s="73" t="s">
+      <c r="I28" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="J28" s="89" t="s">
+      <c r="J28" s="88" t="s">
         <v>106</v>
       </c>
-      <c r="K28" s="76" t="s">
+      <c r="K28" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="L28" s="32"/>
-      <c r="M28" s="85" t="s">
+      <c r="L28" s="31"/>
+      <c r="M28" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="N28" s="84" t="s">
+      <c r="N28" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="O28" s="75" t="s">
+      <c r="O28" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="P28" s="86" t="s">
+      <c r="P28" s="85" t="s">
         <v>112</v>
       </c>
       <c r="Q28" s="22"/>
@@ -2390,7 +2413,7 @@
       <c r="AG28" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="AH28" s="90">
+      <c r="AH28" s="89">
         <v>43831</v>
       </c>
       <c r="AI28" s="22" t="s">
@@ -2403,51 +2426,51 @@
       <c r="AL28" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="AM28" s="59" t="s">
+      <c r="AM28" s="58" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:39" s="39" customFormat="1" ht="14">
-      <c r="A29" s="29">
-        <v>2</v>
-      </c>
-      <c r="B29" s="30" t="s">
+    <row r="29" spans="1:39" s="38" customFormat="1" ht="14">
+      <c r="A29" s="88" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="C29" s="83" t="s">
+      <c r="C29" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="87" t="s">
+      <c r="D29" s="73"/>
+      <c r="E29" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87" t="s">
+      <c r="F29" s="86"/>
+      <c r="G29" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="H29" s="31" t="s">
+      <c r="H29" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="I29" s="88" t="s">
+      <c r="I29" s="87" t="s">
         <v>130</v>
       </c>
-      <c r="J29" s="89" t="s">
+      <c r="J29" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="K29" s="76" t="s">
+      <c r="K29" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="L29" s="32"/>
-      <c r="M29" s="85" t="s">
+      <c r="L29" s="31"/>
+      <c r="M29" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="N29" s="84" t="s">
+      <c r="N29" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="O29" s="75" t="s">
+      <c r="O29" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="P29" s="86" t="s">
+      <c r="P29" s="85" t="s">
         <v>112</v>
       </c>
       <c r="Q29" s="22"/>
@@ -2499,7 +2522,7 @@
       <c r="AG29" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="AH29" s="90">
+      <c r="AH29" s="89">
         <v>43831</v>
       </c>
       <c r="AI29" s="22" t="s">
@@ -2512,53 +2535,53 @@
       <c r="AL29" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="AM29" s="59" t="s">
+      <c r="AM29" s="58" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:39" s="39" customFormat="1" ht="14">
-      <c r="A30" s="29">
-        <v>3</v>
-      </c>
-      <c r="B30" s="30" t="s">
+    <row r="30" spans="1:39" s="38" customFormat="1" ht="14">
+      <c r="A30" s="88" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="C30" s="92" t="s">
+      <c r="C30" s="91" t="s">
         <v>105</v>
       </c>
-      <c r="D30" s="74"/>
-      <c r="E30" s="87" t="s">
+      <c r="D30" s="73"/>
+      <c r="E30" s="86" t="s">
         <v>113</v>
       </c>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87" t="s">
+      <c r="F30" s="86"/>
+      <c r="G30" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="H30" s="31" t="s">
+      <c r="H30" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="I30" s="88" t="s">
+      <c r="I30" s="87" t="s">
         <v>117</v>
       </c>
-      <c r="J30" s="89" t="s">
+      <c r="J30" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="K30" s="76" t="s">
+      <c r="K30" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="L30" s="93" t="s">
+      <c r="L30" s="92" t="s">
         <v>142</v>
       </c>
-      <c r="M30" s="85" t="s">
+      <c r="M30" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="N30" s="84" t="s">
+      <c r="N30" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="O30" s="75" t="s">
+      <c r="O30" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="P30" s="86" t="s">
+      <c r="P30" s="85" t="s">
         <v>112</v>
       </c>
       <c r="Q30" s="22"/>
@@ -2610,7 +2633,7 @@
       <c r="AG30" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="AH30" s="90">
+      <c r="AH30" s="89">
         <v>43831</v>
       </c>
       <c r="AI30" s="22" t="s">
@@ -2625,7 +2648,7 @@
       <c r="AL30" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="AM30" s="59" t="s">
+      <c r="AM30" s="58" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2639,7 +2662,7 @@
       <c r="G31" s="28"/>
       <c r="H31" s="16"/>
       <c r="I31" s="19"/>
-      <c r="J31" s="79"/>
+      <c r="J31" s="78"/>
       <c r="K31" s="26"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
@@ -2679,7 +2702,7 @@
       <c r="G32" s="28"/>
       <c r="H32" s="17"/>
       <c r="I32" s="19"/>
-      <c r="J32" s="79"/>
+      <c r="J32" s="78"/>
       <c r="K32" s="26"/>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
@@ -2719,7 +2742,7 @@
       <c r="G33" s="28"/>
       <c r="H33" s="17"/>
       <c r="I33" s="19"/>
-      <c r="J33" s="79"/>
+      <c r="J33" s="78"/>
       <c r="K33" s="26"/>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
@@ -2759,7 +2782,7 @@
       <c r="G34" s="28"/>
       <c r="H34" s="17"/>
       <c r="I34" s="19"/>
-      <c r="J34" s="79"/>
+      <c r="J34" s="78"/>
       <c r="K34" s="26"/>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
@@ -2799,7 +2822,7 @@
       <c r="G35" s="28"/>
       <c r="H35" s="17"/>
       <c r="I35" s="19"/>
-      <c r="J35" s="79"/>
+      <c r="J35" s="78"/>
       <c r="K35" s="26"/>
       <c r="L35" s="18"/>
       <c r="M35" s="18"/>
@@ -2829,84 +2852,84 @@
       <c r="AK35" s="25"/>
       <c r="AL35" s="25"/>
     </row>
-    <row r="36" spans="1:38" s="34" customFormat="1" ht="14">
-      <c r="A36" s="48"/>
-      <c r="B36" s="47"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="80"/>
-      <c r="K36" s="56"/>
-      <c r="L36" s="52"/>
-      <c r="M36" s="52"/>
-      <c r="N36" s="46"/>
-      <c r="O36" s="51"/>
-      <c r="P36" s="51"/>
-      <c r="Q36" s="53"/>
-      <c r="R36" s="50"/>
-      <c r="S36" s="50"/>
-      <c r="T36" s="53"/>
-      <c r="U36" s="53"/>
-      <c r="V36" s="53"/>
-      <c r="W36" s="35"/>
-      <c r="X36" s="35"/>
-      <c r="Y36" s="35"/>
-      <c r="Z36" s="35"/>
-      <c r="AA36" s="35"/>
-      <c r="AB36" s="35"/>
-      <c r="AC36" s="35"/>
-      <c r="AD36" s="35"/>
-      <c r="AE36" s="35"/>
-      <c r="AF36" s="35"/>
-      <c r="AG36" s="35"/>
-      <c r="AH36" s="35"/>
-      <c r="AI36" s="35"/>
-      <c r="AJ36" s="35"/>
-      <c r="AK36" s="35"/>
-      <c r="AL36" s="35"/>
-    </row>
-    <row r="37" spans="1:38" s="34" customFormat="1" ht="14">
-      <c r="A37" s="45"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="43"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="81"/>
-      <c r="K37" s="57"/>
-      <c r="L37" s="42"/>
-      <c r="M37" s="42"/>
-      <c r="N37" s="43"/>
-      <c r="O37" s="43"/>
-      <c r="P37" s="41"/>
-      <c r="R37" s="40"/>
-      <c r="S37" s="40"/>
-      <c r="W37" s="36"/>
-      <c r="X37" s="36"/>
-      <c r="AA37" s="39"/>
-    </row>
-    <row r="38" spans="1:38" s="34" customFormat="1" ht="14">
-      <c r="A38" s="37"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="41"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="82"/>
-      <c r="K38" s="57"/>
-      <c r="N38" s="41"/>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="R38" s="40"/>
-      <c r="S38" s="40"/>
-      <c r="W38" s="36"/>
-      <c r="X38" s="36"/>
-      <c r="AA38" s="39"/>
+    <row r="36" spans="1:38" s="33" customFormat="1" ht="14">
+      <c r="A36" s="47"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="45"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="52"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
+      <c r="T36" s="52"/>
+      <c r="U36" s="52"/>
+      <c r="V36" s="52"/>
+      <c r="W36" s="34"/>
+      <c r="X36" s="34"/>
+      <c r="Y36" s="34"/>
+      <c r="Z36" s="34"/>
+      <c r="AA36" s="34"/>
+      <c r="AB36" s="34"/>
+      <c r="AC36" s="34"/>
+      <c r="AD36" s="34"/>
+      <c r="AE36" s="34"/>
+      <c r="AF36" s="34"/>
+      <c r="AG36" s="34"/>
+      <c r="AH36" s="34"/>
+      <c r="AI36" s="34"/>
+      <c r="AJ36" s="34"/>
+      <c r="AK36" s="34"/>
+      <c r="AL36" s="34"/>
+    </row>
+    <row r="37" spans="1:38" s="33" customFormat="1" ht="14">
+      <c r="A37" s="44"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="42"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="80"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="41"/>
+      <c r="M37" s="41"/>
+      <c r="N37" s="42"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="40"/>
+      <c r="R37" s="39"/>
+      <c r="S37" s="39"/>
+      <c r="W37" s="35"/>
+      <c r="X37" s="35"/>
+      <c r="AA37" s="38"/>
+    </row>
+    <row r="38" spans="1:38" s="33" customFormat="1" ht="14">
+      <c r="A38" s="36"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="81"/>
+      <c r="K38" s="56"/>
+      <c r="N38" s="40"/>
+      <c r="O38" s="40"/>
+      <c r="P38" s="40"/>
+      <c r="R38" s="39"/>
+      <c r="S38" s="39"/>
+      <c r="W38" s="35"/>
+      <c r="X38" s="35"/>
+      <c r="AA38" s="38"/>
     </row>
     <row r="39" spans="1:38">
-      <c r="A39" s="37"/>
+      <c r="A39" s="36"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -3032,7 +3055,7 @@
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="72" t="s">
+      <c r="E12" s="71" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3040,7 +3063,7 @@
       <c r="A13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="72" t="s">
+      <c r="E13" s="71" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3048,7 +3071,7 @@
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="58" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3064,15 +3087,15 @@
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="58" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="38" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>